<commit_message>
Adicionado busca e status vermelho
</commit_message>
<xml_diff>
--- a/lista de convidados.xlsx
+++ b/lista de convidados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacao\Sites\Programa Loja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CACE63-54E2-4042-AB4F-F4B20195D529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1B4DA8-BA06-403D-B734-60C709B2AD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Larissa </t>
   </si>
@@ -40,6 +40,42 @@
   </si>
   <si>
     <t>mesa</t>
+  </si>
+  <si>
+    <t>lucas</t>
+  </si>
+  <si>
+    <t>maria</t>
+  </si>
+  <si>
+    <t>natalia</t>
+  </si>
+  <si>
+    <t>manuaela</t>
+  </si>
+  <si>
+    <t>manuela</t>
+  </si>
+  <si>
+    <t>pedro</t>
+  </si>
+  <si>
+    <t>joao</t>
+  </si>
+  <si>
+    <t>ronal</t>
+  </si>
+  <si>
+    <t>francisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">junior </t>
+  </si>
+  <si>
+    <t>felipe</t>
+  </si>
+  <si>
+    <t>patricia</t>
   </si>
 </sst>
 </file>
@@ -369,7 +405,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,8 +445,101 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P23" s="1"/>

</xml_diff>